<commit_message>
pagina de ayuda ajax
</commit_message>
<xml_diff>
--- a/Control Rosalis.xlsx
+++ b/Control Rosalis.xlsx
@@ -847,8 +847,11 @@
                 <c:pt idx="4">
                   <c:v>155.94999999999999</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
                 <c:pt idx="6">
-                  <c:v>1540</c:v>
+                  <c:v>2240</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1030</c:v>
@@ -860,7 +863,7 @@
                   <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4841.4799999999996</c:v>
+                  <c:v>5234.4799999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12000</c:v>
@@ -879,11 +882,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="181294592"/>
-        <c:axId val="181296128"/>
+        <c:axId val="190797312"/>
+        <c:axId val="190798848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181294592"/>
+        <c:axId val="190797312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,7 +895,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181296128"/>
+        <c:crossAx val="190798848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -900,7 +903,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181296128"/>
+        <c:axId val="190798848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,7 +914,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181294592"/>
+        <c:crossAx val="190797312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1076,11 +1079,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="181641216"/>
-        <c:axId val="181642752"/>
+        <c:axId val="191078400"/>
+        <c:axId val="191079936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181641216"/>
+        <c:axId val="191078400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,7 +1092,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181642752"/>
+        <c:crossAx val="191079936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1097,7 +1100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181642752"/>
+        <c:axId val="191079936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1108,7 +1111,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181641216"/>
+        <c:crossAx val="191078400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1487,7 +1490,7 @@
   <dimension ref="B2:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="H13:I15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,7 +1675,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,7 +1752,9 @@
       <c r="B7" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="34">
+        <v>3000</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
@@ -1757,7 +1762,7 @@
         <v>36</v>
       </c>
       <c r="C8" s="34">
-        <v>1540</v>
+        <v>2240</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1801,7 +1806,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="36">
-        <v>4841.4799999999996</v>
+        <v>5234.4799999999996</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="0.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1818,7 +1823,7 @@
       </c>
       <c r="C14" s="38">
         <f>SUM(C2:C12)</f>
-        <v>12089.939999999999</v>
+        <v>16182.939999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
230119 ajuste salario adelson
</commit_message>
<xml_diff>
--- a/Control Rosalis.xlsx
+++ b/Control Rosalis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="Enero" sheetId="5" r:id="rId2"/>
     <sheet name="Diciembre año pasado" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>Ingresos</t>
   </si>
@@ -160,12 +160,15 @@
   </si>
   <si>
     <t>Gastos V</t>
+  </si>
+  <si>
+    <t>Otros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -234,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,8 +298,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -555,6 +564,19 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -565,7 +587,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
@@ -587,7 +609,6 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -605,18 +626,6 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -631,21 +640,36 @@
     <xf numFmtId="43" fontId="3" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="3" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="2" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="2" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="10" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="11" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -666,14 +690,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-DO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -704,6 +731,11 @@
                 <a:srgbClr val="68E945"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F86B-4F8D-A749-945F9421E404}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -717,6 +749,11 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F86B-4F8D-A749-945F9421E404}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -727,6 +764,11 @@
                 <a:srgbClr val="68E945"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F86B-4F8D-A749-945F9421E404}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -740,6 +782,11 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-F86B-4F8D-A749-945F9421E404}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -750,6 +797,11 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-F86B-4F8D-A749-945F9421E404}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -763,6 +815,11 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-F86B-4F8D-A749-945F9421E404}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -773,6 +830,11 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-F86B-4F8D-A749-945F9421E404}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -786,6 +848,11 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-F86B-4F8D-A749-945F9421E404}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -826,10 +893,10 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>69828.399999999994</c:v>
+                  <c:v>69798.23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20608.400000000001</c:v>
+                  <c:v>20638.57</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>50000</c:v>
@@ -852,9 +919,13 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-F86B-4F8D-A749-945F9421E404}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -873,6 +944,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -913,9 +985,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-DO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -942,7 +1014,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -957,6 +1028,13 @@
           <c:order val="0"/>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -965,6 +1043,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1049,6 +1132,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0168-40B7-9B74-64E6A6D46F8E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1070,6 +1158,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1222,7 +1311,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1257,7 +1346,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1481,34 +1570,34 @@
   <sheetData>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24">
+      <c r="C4" s="23"/>
+      <c r="D4" s="23">
         <v>1</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>2</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>3</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="23">
         <v>4</v>
       </c>
       <c r="H4" s="1"/>
@@ -1518,112 +1607,112 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="27">
         <v>302456.55</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="27">
         <v>549.48</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="26">
         <v>804912</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <v>9310.41</v>
       </c>
-      <c r="G5" s="28"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="29">
         <v>69.77</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="29">
         <v>-3.73</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="28">
         <v>-3.73</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="29">
         <v>-3.73</v>
       </c>
-      <c r="G6" s="30"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="29">
         <v>6080.14</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="29">
         <v>5210.1400000000003</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="28">
         <v>2506.66</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="29">
         <v>2521.6799999999998</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="29">
         <v>3666.33</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <v>26.33</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="28">
         <v>26.33</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="29">
         <v>9.8000000000000007</v>
       </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="29"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="28">
         <v>550</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="29">
         <v>800</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="28">
         <v>100</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="29">
         <v>900</v>
       </c>
-      <c r="G9" s="30"/>
+      <c r="G9" s="29"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="24">
         <v>4928</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="25">
         <v>3060</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <v>3003</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="25">
         <v>297</v>
       </c>
-      <c r="G10" s="26"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
@@ -1666,7 +1755,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,7 +1765,7 @@
     <col min="3" max="3" width="12.42578125" style="12" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="41" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -1686,51 +1775,51 @@
         <v>33</v>
       </c>
       <c r="C1" s="50"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37">
-        <f>SUM(H8:H12)</f>
-        <v>69828.399999999994</v>
+      <c r="C2" s="32">
+        <f>SUM(H8:H13)</f>
+        <v>69798.23</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="34">
         <f>H4</f>
         <v>50000</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="44" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="37">
         <f>SUM(D8:D13)</f>
         <v>15413.53</v>
       </c>
@@ -1738,19 +1827,19 @@
       <c r="F4" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="54">
         <v>0</v>
       </c>
-      <c r="H4" s="55">
+      <c r="H4" s="45">
         <v>50000</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="37">
         <v>4414.87</v>
       </c>
     </row>
@@ -1760,22 +1849,22 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="44" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1784,20 +1873,20 @@
       <c r="B8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="54">
         <v>1235</v>
       </c>
-      <c r="D8" s="55">
+      <c r="D8" s="45">
         <v>1235</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="54">
         <v>0</v>
       </c>
-      <c r="H8" s="55">
-        <v>49220</v>
+      <c r="H8" s="45">
+        <v>49189.83</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -1806,19 +1895,19 @@
       <c r="B9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="54">
         <v>0</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="45">
         <v>900</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="54">
         <v>7304.2</v>
       </c>
-      <c r="H9" s="55">
+      <c r="H9" s="45">
         <v>7304.2</v>
       </c>
     </row>
@@ -1827,40 +1916,40 @@
       <c r="B10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="54">
         <v>1800</v>
       </c>
-      <c r="D10" s="55">
+      <c r="D10" s="45">
         <v>1800</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="54">
         <v>7304.2</v>
       </c>
-      <c r="H10" s="55">
+      <c r="H10" s="45">
         <v>7304.2</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C11" s="54">
         <v>0</v>
       </c>
-      <c r="D11" s="55">
+      <c r="D11" s="45">
         <v>200</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="45">
+      <c r="G11" s="54">
         <v>3500</v>
       </c>
-      <c r="H11" s="55">
+      <c r="H11" s="45">
         <v>3500</v>
       </c>
     </row>
@@ -1869,19 +1958,19 @@
       <c r="B12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="54">
         <v>1800</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="45">
         <v>2400</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="55">
         <v>2500</v>
       </c>
-      <c r="H12" s="55">
+      <c r="H12" s="53">
         <v>2500</v>
       </c>
     </row>
@@ -1889,270 +1978,279 @@
       <c r="B13" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="54">
         <v>8878.5300000000007</v>
       </c>
-      <c r="D13" s="55">
+      <c r="D13" s="45">
         <v>8878.5300000000007</v>
+      </c>
+      <c r="F13" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="55">
+        <v>30.17</v>
+      </c>
+      <c r="H13" s="53">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="35"/>
+      <c r="H15" s="30"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C16" s="56">
         <v>205</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="49">
+      <c r="C17" s="56">
         <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="49">
+      <c r="C18" s="56">
         <v>50</v>
       </c>
-      <c r="H18" s="35"/>
+      <c r="H18" s="30"/>
     </row>
     <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="49">
+      <c r="C19" s="56">
         <v>907.07</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="49">
+      <c r="C20" s="56">
         <v>237.29</v>
       </c>
       <c r="I20" s="12"/>
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="49">
+      <c r="C21" s="56">
         <v>300</v>
       </c>
       <c r="I21" s="12"/>
     </row>
     <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C22" s="56">
         <v>1090</v>
       </c>
       <c r="I22" s="12"/>
     </row>
     <row r="23" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="51">
+      <c r="C23" s="57">
         <v>1524.29</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="51">
+      <c r="C24" s="57">
         <v>690</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="40"/>
-      <c r="C25" s="51"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="57"/>
     </row>
     <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="40"/>
-      <c r="C26" s="49"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="56"/>
     </row>
     <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="40"/>
-      <c r="C27" s="49"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="56"/>
     </row>
     <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="40"/>
-      <c r="C28" s="49"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="56"/>
     </row>
     <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="40"/>
-      <c r="C29" s="49"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="56"/>
     </row>
     <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="40"/>
-      <c r="C30" s="49"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="56"/>
     </row>
     <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="40"/>
-      <c r="C31" s="49"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="56"/>
     </row>
     <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="40"/>
-      <c r="C32" s="49"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="56"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="40"/>
-      <c r="C33" s="49"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="56"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="40"/>
-      <c r="C34" s="49"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="56"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="40"/>
-      <c r="C35" s="49"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="56"/>
     </row>
     <row r="36" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="40"/>
-      <c r="C36" s="49"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="56"/>
     </row>
     <row r="37" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="40"/>
-      <c r="C37" s="49"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="56"/>
     </row>
     <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="40"/>
-      <c r="C38" s="49"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="56"/>
     </row>
     <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="40"/>
-      <c r="C39" s="49"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="56"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="40"/>
-      <c r="C40" s="49"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="56"/>
     </row>
     <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="40"/>
-      <c r="C41" s="49"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="56"/>
     </row>
     <row r="42" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="40"/>
-      <c r="C42" s="49"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="56"/>
     </row>
     <row r="43" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="40"/>
-      <c r="C43" s="49"/>
-      <c r="F43" s="47" t="s">
+      <c r="B43" s="35"/>
+      <c r="C43" s="56"/>
+      <c r="F43" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="G43" s="35">
+      <c r="G43" s="30">
         <f>C2</f>
-        <v>69828.399999999994</v>
+        <v>69798.23</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="40"/>
-      <c r="C44" s="49"/>
-      <c r="F44" s="47" t="s">
+      <c r="B44" s="35"/>
+      <c r="C44" s="56"/>
+      <c r="F44" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G44" s="35">
-        <f>SUM(G8:G12)</f>
-        <v>20608.400000000001</v>
+      <c r="G44" s="30">
+        <f>SUM(G8:G13)</f>
+        <v>20638.57</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="40"/>
-      <c r="C45" s="49"/>
-      <c r="F45" s="47" t="s">
+      <c r="B45" s="35"/>
+      <c r="C45" s="56"/>
+      <c r="F45" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="G45" s="35">
+      <c r="G45" s="30">
         <f>H4</f>
         <v>50000</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="40"/>
-      <c r="C46" s="49"/>
-      <c r="F46" s="47" t="s">
+      <c r="B46" s="35"/>
+      <c r="C46" s="56"/>
+      <c r="F46" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G46" s="35">
+      <c r="G46" s="30">
         <f>G4</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="40"/>
-      <c r="C47" s="49"/>
-      <c r="F47" s="47" t="s">
+      <c r="B47" s="35"/>
+      <c r="C47" s="56"/>
+      <c r="F47" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="G47" s="35">
+      <c r="G47" s="30">
         <f>C4</f>
         <v>15413.53</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="40"/>
-      <c r="C48" s="49"/>
-      <c r="F48" s="47" t="s">
+      <c r="B48" s="35"/>
+      <c r="C48" s="56"/>
+      <c r="F48" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G48" s="35">
+      <c r="G48" s="30">
         <f>SUM(C8:C13)</f>
         <v>13713.53</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="40"/>
-      <c r="C49" s="49"/>
-      <c r="F49" s="47" t="s">
+      <c r="B49" s="35"/>
+      <c r="C49" s="56"/>
+      <c r="F49" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="G49" s="35">
+      <c r="G49" s="30">
         <f>C5</f>
         <v>4414.87</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="40"/>
-      <c r="C50" s="49"/>
-      <c r="F50" s="47" t="s">
+      <c r="B50" s="35"/>
+      <c r="C50" s="56"/>
+      <c r="F50" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G50" s="35">
+      <c r="G50" s="30">
         <f>SUM(C16:C120)</f>
         <v>5143.6499999999996</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="40"/>
-      <c r="C51" s="49"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="56"/>
     </row>
     <row r="52" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="40"/>
-      <c r="C52" s="49"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="56"/>
     </row>
     <row r="53" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="40"/>
-      <c r="C53" s="49"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
cuentas contables y prestamos normalizado
</commit_message>
<xml_diff>
--- a/Control Rosalis.xlsx
+++ b/Control Rosalis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
@@ -12,12 +12,12 @@
     <sheet name="Inventario" sheetId="2" r:id="rId3"/>
     <sheet name="Febrero" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="102">
   <si>
     <t>Ingresos</t>
   </si>
@@ -320,12 +320,15 @@
   </si>
   <si>
     <t>maiz palomita</t>
+  </si>
+  <si>
+    <t>ADELSON PRESTAMOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -793,9 +796,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-DO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -826,7 +829,7 @@
                 <a:srgbClr val="68E945"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -844,7 +847,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -859,7 +862,7 @@
                 <a:srgbClr val="68E945"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -877,7 +880,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -892,7 +895,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -910,7 +913,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -969,7 +972,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-3FA8-4974-82FB-960EC423E8D0}"/>
             </c:ext>
@@ -1035,9 +1038,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-DO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1093,7 +1096,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1182,7 +1185,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DC0B-40CC-97AB-203C2039427D}"/>
             </c:ext>
@@ -1249,9 +1252,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-DO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1282,7 +1285,7 @@
                 <a:srgbClr val="68E945"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -1300,7 +1303,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -1315,7 +1318,7 @@
                 <a:srgbClr val="68E945"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -1333,7 +1336,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -1348,7 +1351,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -1366,7 +1369,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-3FA8-4974-82FB-960EC423E8D0}"/>
               </c:ext>
@@ -1425,7 +1428,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-3FA8-4974-82FB-960EC423E8D0}"/>
             </c:ext>
@@ -1640,7 +1643,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1675,7 +1678,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3118,10 +3121,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J22"/>
+  <dimension ref="A3:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3359,10 +3362,10 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
       <c r="B17" s="50" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C17" s="47">
-        <v>50063.15</v>
+        <v>3000</v>
       </c>
       <c r="D17" s="47"/>
       <c r="E17" s="47"/>
@@ -3372,10 +3375,10 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="50" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="C18" s="47">
-        <v>205.34</v>
+        <v>50063.15</v>
       </c>
       <c r="D18" s="47"/>
       <c r="E18" s="47"/>
@@ -3385,10 +3388,10 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="50" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19" s="47">
-        <v>4.4400000000000004</v>
+        <v>205.34</v>
       </c>
       <c r="D19" s="47"/>
       <c r="E19" s="47"/>
@@ -3397,45 +3400,58 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="44"/>
-      <c r="B20" s="51" t="s">
-        <v>66</v>
+      <c r="B20" s="50" t="s">
+        <v>7</v>
       </c>
       <c r="C20" s="47">
-        <v>300</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="D20" s="47"/>
       <c r="E20" s="47"/>
       <c r="F20" s="47"/>
       <c r="G20" s="44"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="44"/>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="47">
+        <v>300</v>
+      </c>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="44"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="44"/>
+      <c r="B22" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C22" s="48">
         <v>610</v>
       </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="44"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
       <c r="G22" s="44"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C13:F13"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:E10 C15:E21">
+  <conditionalFormatting sqref="C5:E10 C15:E22">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3449,7 +3465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B10" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
contabilidad, comision , cuadre e inventario
</commit_message>
<xml_diff>
--- a/Control Rosalis.xlsx
+++ b/Control Rosalis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Enero" sheetId="5" r:id="rId1"/>
@@ -1185,11 +1185,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="49487872"/>
-        <c:axId val="49489408"/>
+        <c:axId val="132700032"/>
+        <c:axId val="132701568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49487872"/>
+        <c:axId val="132700032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,7 +1199,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49489408"/>
+        <c:crossAx val="132701568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1207,7 +1207,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49489408"/>
+        <c:axId val="132701568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1218,7 +1218,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49487872"/>
+        <c:crossAx val="132700032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1399,11 +1399,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="49710976"/>
-        <c:axId val="49712512"/>
+        <c:axId val="162533376"/>
+        <c:axId val="162534912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49710976"/>
+        <c:axId val="162533376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,7 +1413,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49712512"/>
+        <c:crossAx val="162534912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1421,7 +1421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49712512"/>
+        <c:axId val="162534912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1432,7 +1432,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49710976"/>
+        <c:crossAx val="162533376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1641,11 +1641,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="223113984"/>
-        <c:axId val="223115520"/>
+        <c:axId val="159042176"/>
+        <c:axId val="159043968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="223113984"/>
+        <c:axId val="159042176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1655,7 +1655,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223115520"/>
+        <c:crossAx val="159043968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1663,7 +1663,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="223115520"/>
+        <c:axId val="159043968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,7 +1674,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223113984"/>
+        <c:crossAx val="159042176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3333,7 +3333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -3723,8 +3723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B76" workbookViewId="0">
+      <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
contabilidad mysql y sql
</commit_message>
<xml_diff>
--- a/Control Rosalis.xlsx
+++ b/Control Rosalis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Enero" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="200">
   <si>
     <t>Ingresos</t>
   </si>
@@ -592,6 +592,33 @@
   </si>
   <si>
     <t>10.26-</t>
+  </si>
+  <si>
+    <t>tarjeta cas</t>
+  </si>
+  <si>
+    <t>habichuela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naranja </t>
+  </si>
+  <si>
+    <t>verdura</t>
+  </si>
+  <si>
+    <t>molondrones</t>
+  </si>
+  <si>
+    <t>adel yogur</t>
+  </si>
+  <si>
+    <t>comida adel</t>
+  </si>
+  <si>
+    <t>adelyogur</t>
+  </si>
+  <si>
+    <t>salami huevo</t>
   </si>
 </sst>
 </file>
@@ -1276,11 +1303,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="181734016"/>
-        <c:axId val="181735808"/>
+        <c:axId val="181406336"/>
+        <c:axId val="181408128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181734016"/>
+        <c:axId val="181406336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1290,7 +1317,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181735808"/>
+        <c:crossAx val="181408128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1298,7 +1325,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181735808"/>
+        <c:axId val="181408128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,7 +1336,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181734016"/>
+        <c:crossAx val="181406336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1490,11 +1517,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="182080256"/>
-        <c:axId val="182081792"/>
+        <c:axId val="181818112"/>
+        <c:axId val="181819648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182080256"/>
+        <c:axId val="181818112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,7 +1531,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182081792"/>
+        <c:crossAx val="181819648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1512,7 +1539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182081792"/>
+        <c:axId val="181819648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1523,7 +1550,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182080256"/>
+        <c:crossAx val="181818112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1732,11 +1759,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182168960"/>
-        <c:axId val="182170752"/>
+        <c:axId val="181775744"/>
+        <c:axId val="181777536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182168960"/>
+        <c:axId val="181775744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1746,7 +1773,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182170752"/>
+        <c:crossAx val="181777536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1754,7 +1781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182170752"/>
+        <c:axId val="181777536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1765,7 +1792,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182168960"/>
+        <c:crossAx val="181775744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1974,11 +2001,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182347648"/>
-        <c:axId val="182349184"/>
+        <c:axId val="182015872"/>
+        <c:axId val="182017408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182347648"/>
+        <c:axId val="182015872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1988,7 +2015,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182349184"/>
+        <c:crossAx val="182017408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1996,7 +2023,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182349184"/>
+        <c:axId val="182017408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2007,7 +2034,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182347648"/>
+        <c:crossAx val="182015872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2458,7 +2485,7 @@
   <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N32" sqref="B1:N32"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4093,8 +4120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView showGridLines="0" topLeftCell="B103" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5461,10 +5488,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V113"/>
+  <dimension ref="B1:V140"/>
   <sheetViews>
-    <sheetView topLeftCell="M4" workbookViewId="0">
-      <selection activeCell="W33" sqref="W33"/>
+    <sheetView tabSelected="1" topLeftCell="M43" workbookViewId="0">
+      <selection activeCell="O60" sqref="O60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5482,7 +5509,7 @@
     <col min="11" max="11" width="13" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" customWidth="1"/>
     <col min="13" max="13" width="23.42578125" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" customWidth="1"/>
     <col min="16" max="16" width="6" customWidth="1"/>
     <col min="17" max="17" width="20.85546875" customWidth="1"/>
@@ -5518,8 +5545,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="21">
-        <f>SUM(S9:S13)</f>
-        <v>69798.23</v>
+        <v>69838.23</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="60"/>
@@ -5593,8 +5619,7 @@
         <v>34</v>
       </c>
       <c r="N6" s="37">
-        <f>N3-(N4+N5)</f>
-        <v>5623.2299999999959</v>
+        <v>5663.23</v>
       </c>
       <c r="Q6" s="30"/>
     </row>
@@ -5607,6 +5632,15 @@
         <v>14175</v>
       </c>
       <c r="F7" s="3"/>
+      <c r="Q7" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="35" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="25" t="s">
@@ -5621,15 +5655,14 @@
       </c>
       <c r="N8" s="62"/>
       <c r="O8" s="62"/>
-      <c r="Q8" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="R8" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="S8" s="35" t="s">
-        <v>37</v>
-      </c>
+      <c r="Q8" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" s="18"/>
+      <c r="S8" s="36">
+        <v>49189.83</v>
+      </c>
+      <c r="T8" s="1"/>
     </row>
     <row r="9" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M9" s="34" t="s">
@@ -5642,13 +5675,14 @@
         <v>37</v>
       </c>
       <c r="Q9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="R9" s="18"/>
+        <v>39</v>
+      </c>
+      <c r="R9" s="18">
+        <v>7324.2</v>
+      </c>
       <c r="S9" s="36">
-        <v>49189.83</v>
-      </c>
-      <c r="T9" s="1"/>
+        <v>7324.2</v>
+      </c>
     </row>
     <row r="10" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="56" t="s">
@@ -5664,11 +5698,11 @@
         <v>1235</v>
       </c>
       <c r="Q10" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R10" s="18"/>
       <c r="S10" s="36">
-        <v>7304.2</v>
+        <v>7324.2</v>
       </c>
     </row>
     <row r="11" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5690,12 +5724,12 @@
       <c r="O11" s="36">
         <v>900</v>
       </c>
-      <c r="Q11" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="R11" s="18"/>
+      <c r="Q11" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="R11" s="28"/>
       <c r="S11" s="36">
-        <v>7304.2</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="12" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5717,12 +5751,12 @@
       <c r="O12" s="36">
         <v>1800</v>
       </c>
-      <c r="Q12" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="R12" s="28"/>
+      <c r="Q12" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="R12" s="18"/>
       <c r="S12" s="36">
-        <v>3500</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="13" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5745,11 +5779,13 @@
         <v>190</v>
       </c>
       <c r="Q13" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="R13" s="18"/>
+        <v>86</v>
+      </c>
+      <c r="R13" s="18">
+        <v>780</v>
+      </c>
       <c r="S13" s="36">
-        <v>2500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5817,8 +5853,8 @@
         <v>56</v>
       </c>
       <c r="R16" s="41">
-        <f>SUM(R18:R222)</f>
-        <v>1508.4299999999998</v>
+        <f>SUM(R18:R249)</f>
+        <v>1731.4299999999998</v>
       </c>
     </row>
     <row r="17" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5905,8 +5941,8 @@
         <v>59</v>
       </c>
       <c r="N20" s="41">
-        <f>SUM(N22:N222)</f>
-        <v>2134</v>
+        <f>SUM(N22:N249)</f>
+        <v>2983.27</v>
       </c>
       <c r="Q20" s="29" t="s">
         <v>114</v>
@@ -6057,7 +6093,7 @@
       </c>
       <c r="V27" s="19">
         <f>N3</f>
-        <v>69798.23</v>
+        <v>69838.23</v>
       </c>
     </row>
     <row r="28" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6082,10 +6118,7 @@
       <c r="U28" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="V28" s="19">
-        <f>SUM(R9:R13)</f>
-        <v>0</v>
-      </c>
+      <c r="V28" s="19"/>
     </row>
     <row r="29" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="24" t="s">
@@ -6246,8 +6279,12 @@
       <c r="N36" s="32">
         <v>65</v>
       </c>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="33"/>
+      <c r="Q36" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="R36" s="33">
+        <v>10</v>
+      </c>
       <c r="U36" s="30"/>
       <c r="V36" s="19"/>
     </row>
@@ -6264,8 +6301,12 @@
       <c r="N37" s="32">
         <v>100</v>
       </c>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="33"/>
+      <c r="Q37" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="R37" s="33">
+        <v>40</v>
+      </c>
       <c r="U37" s="30" t="s">
         <v>35</v>
       </c>
@@ -6280,8 +6321,12 @@
       <c r="N38" s="32">
         <v>125</v>
       </c>
-      <c r="Q38" s="24"/>
-      <c r="R38" s="33"/>
+      <c r="Q38" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="R38" s="33">
+        <v>70</v>
+      </c>
       <c r="U38" s="30"/>
       <c r="V38" s="19"/>
     </row>
@@ -6294,8 +6339,12 @@
       <c r="N39" s="32">
         <v>50</v>
       </c>
-      <c r="Q39" s="24"/>
-      <c r="R39" s="33"/>
+      <c r="Q39" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="R39" s="33">
+        <v>70</v>
+      </c>
       <c r="U39" s="30"/>
       <c r="V39" s="19"/>
     </row>
@@ -6308,8 +6357,12 @@
       <c r="N40" s="32">
         <v>20</v>
       </c>
-      <c r="Q40" s="24"/>
-      <c r="R40" s="33"/>
+      <c r="Q40" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="R40" s="33">
+        <v>8</v>
+      </c>
       <c r="U40" s="30"/>
       <c r="V40" s="19"/>
     </row>
@@ -6322,8 +6375,12 @@
       <c r="N41" s="32">
         <v>74</v>
       </c>
-      <c r="Q41" s="24"/>
-      <c r="R41" s="33"/>
+      <c r="Q41" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="R41" s="33">
+        <v>25</v>
+      </c>
       <c r="U41" s="30"/>
       <c r="V41" s="19"/>
     </row>
@@ -6414,8 +6471,12 @@
     <row r="48" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D48" s="24"/>
       <c r="E48" s="32"/>
-      <c r="M48" s="24"/>
-      <c r="N48" s="32"/>
+      <c r="M48" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="N48" s="32">
+        <v>39.74</v>
+      </c>
       <c r="Q48" s="24"/>
       <c r="R48" s="33"/>
       <c r="U48" s="30"/>
@@ -6424,8 +6485,12 @@
     <row r="49" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="24"/>
       <c r="E49" s="32"/>
-      <c r="M49" s="24"/>
-      <c r="N49" s="32"/>
+      <c r="M49" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="N49" s="32">
+        <v>50</v>
+      </c>
       <c r="Q49" s="24"/>
       <c r="R49" s="33"/>
       <c r="U49" s="30"/>
@@ -6434,8 +6499,12 @@
     <row r="50" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="24"/>
       <c r="E50" s="32"/>
-      <c r="M50" s="24"/>
-      <c r="N50" s="32"/>
+      <c r="M50" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="N50" s="32">
+        <v>20</v>
+      </c>
       <c r="Q50" s="24"/>
       <c r="R50" s="33"/>
       <c r="U50" s="30"/>
@@ -6444,8 +6513,12 @@
     <row r="51" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="24"/>
       <c r="E51" s="32"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="32"/>
+      <c r="M51" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="N51" s="32">
+        <v>50</v>
+      </c>
       <c r="Q51" s="24"/>
       <c r="R51" s="33"/>
       <c r="U51" s="30"/>
@@ -6454,360 +6527,451 @@
     <row r="52" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="24"/>
       <c r="E52" s="32"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="32"/>
+      <c r="M52" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="N52" s="32">
+        <v>10</v>
+      </c>
       <c r="Q52" s="24"/>
       <c r="R52" s="33"/>
       <c r="U52" s="30"/>
       <c r="V52" s="19"/>
     </row>
     <row r="53" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E53" s="32">
-        <v>5</v>
-      </c>
-      <c r="M53" s="24"/>
-      <c r="N53" s="32"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="32"/>
+      <c r="M53" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="N53" s="32">
+        <v>20</v>
+      </c>
       <c r="Q53" s="24"/>
       <c r="R53" s="33"/>
+      <c r="U53" s="30"/>
+      <c r="V53" s="19"/>
     </row>
     <row r="54" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E54" s="32">
-        <v>65</v>
-      </c>
+      <c r="D54" s="24"/>
+      <c r="E54" s="32"/>
+      <c r="M54" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="N54" s="32">
+        <v>156.82</v>
+      </c>
+      <c r="Q54" s="24"/>
+      <c r="R54" s="33"/>
+      <c r="U54" s="30"/>
+      <c r="V54" s="19"/>
     </row>
     <row r="55" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D55" s="24"/>
       <c r="E55" s="32"/>
+      <c r="M55" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="N55" s="32">
+        <v>122.71</v>
+      </c>
+      <c r="Q55" s="24"/>
+      <c r="R55" s="33"/>
+      <c r="U55" s="30"/>
+      <c r="V55" s="19"/>
     </row>
     <row r="56" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="24" t="s">
+      <c r="D56" s="24"/>
+      <c r="E56" s="32"/>
+      <c r="M56" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="N56" s="32">
+        <v>45</v>
+      </c>
+      <c r="Q56" s="24"/>
+      <c r="R56" s="33"/>
+      <c r="U56" s="30"/>
+      <c r="V56" s="19"/>
+    </row>
+    <row r="57" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D57" s="24"/>
+      <c r="E57" s="32"/>
+      <c r="M57" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="N57" s="32">
+        <v>150</v>
+      </c>
+      <c r="Q57" s="24"/>
+      <c r="R57" s="33"/>
+      <c r="U57" s="30"/>
+      <c r="V57" s="19"/>
+    </row>
+    <row r="58" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D58" s="24"/>
+      <c r="E58" s="32"/>
+      <c r="M58" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="N58" s="32">
+        <v>15</v>
+      </c>
+      <c r="Q58" s="24"/>
+      <c r="R58" s="33"/>
+      <c r="U58" s="30"/>
+      <c r="V58" s="19"/>
+    </row>
+    <row r="59" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="24"/>
+      <c r="E59" s="32"/>
+      <c r="M59" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="N59" s="32">
+        <v>60</v>
+      </c>
+      <c r="Q59" s="24"/>
+      <c r="R59" s="33"/>
+      <c r="U59" s="30"/>
+      <c r="V59" s="19"/>
+    </row>
+    <row r="60" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="24"/>
+      <c r="E60" s="32"/>
+      <c r="M60" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="N60" s="32">
+        <v>110</v>
+      </c>
+      <c r="Q60" s="24"/>
+      <c r="R60" s="33"/>
+      <c r="U60" s="30"/>
+      <c r="V60" s="19"/>
+    </row>
+    <row r="61" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D61" s="24"/>
+      <c r="E61" s="32"/>
+      <c r="M61" s="24"/>
+      <c r="N61" s="32"/>
+      <c r="Q61" s="24"/>
+      <c r="R61" s="33"/>
+      <c r="U61" s="30"/>
+      <c r="V61" s="19"/>
+    </row>
+    <row r="62" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D62" s="24"/>
+      <c r="E62" s="32"/>
+      <c r="M62" s="24"/>
+      <c r="N62" s="32"/>
+      <c r="Q62" s="24"/>
+      <c r="R62" s="33"/>
+      <c r="U62" s="30"/>
+      <c r="V62" s="19"/>
+    </row>
+    <row r="63" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D63" s="24"/>
+      <c r="E63" s="32"/>
+      <c r="M63" s="24"/>
+      <c r="N63" s="32"/>
+      <c r="Q63" s="24"/>
+      <c r="R63" s="33"/>
+      <c r="U63" s="30"/>
+      <c r="V63" s="19"/>
+    </row>
+    <row r="64" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D64" s="24"/>
+      <c r="E64" s="32"/>
+      <c r="M64" s="24"/>
+      <c r="N64" s="32"/>
+      <c r="Q64" s="24"/>
+      <c r="R64" s="33"/>
+      <c r="U64" s="30"/>
+      <c r="V64" s="19"/>
+    </row>
+    <row r="65" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D65" s="24"/>
+      <c r="E65" s="32"/>
+      <c r="M65" s="24"/>
+      <c r="N65" s="32"/>
+      <c r="Q65" s="24"/>
+      <c r="R65" s="33"/>
+      <c r="U65" s="30"/>
+      <c r="V65" s="19"/>
+    </row>
+    <row r="66" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D66" s="24"/>
+      <c r="E66" s="32"/>
+      <c r="M66" s="24"/>
+      <c r="N66" s="32"/>
+      <c r="Q66" s="24"/>
+      <c r="R66" s="33"/>
+      <c r="U66" s="30"/>
+      <c r="V66" s="19"/>
+    </row>
+    <row r="67" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D67" s="24"/>
+      <c r="E67" s="32"/>
+      <c r="M67" s="24"/>
+      <c r="N67" s="32"/>
+      <c r="Q67" s="24"/>
+      <c r="R67" s="33"/>
+      <c r="U67" s="30"/>
+      <c r="V67" s="19"/>
+    </row>
+    <row r="68" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D68" s="24"/>
+      <c r="E68" s="32"/>
+      <c r="M68" s="24"/>
+      <c r="N68" s="32"/>
+      <c r="Q68" s="24"/>
+      <c r="R68" s="33"/>
+      <c r="U68" s="30"/>
+      <c r="V68" s="19"/>
+    </row>
+    <row r="69" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D69" s="24"/>
+      <c r="E69" s="32"/>
+      <c r="M69" s="24"/>
+      <c r="N69" s="32"/>
+      <c r="Q69" s="24"/>
+      <c r="R69" s="33"/>
+      <c r="U69" s="30"/>
+      <c r="V69" s="19"/>
+    </row>
+    <row r="70" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D70" s="24"/>
+      <c r="E70" s="32"/>
+      <c r="M70" s="24"/>
+      <c r="N70" s="32"/>
+      <c r="Q70" s="24"/>
+      <c r="R70" s="33"/>
+      <c r="U70" s="30"/>
+      <c r="V70" s="19"/>
+    </row>
+    <row r="71" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D71" s="24"/>
+      <c r="E71" s="32"/>
+      <c r="M71" s="24"/>
+      <c r="N71" s="32"/>
+      <c r="Q71" s="24"/>
+      <c r="R71" s="33"/>
+      <c r="U71" s="30"/>
+      <c r="V71" s="19"/>
+    </row>
+    <row r="72" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D72" s="24"/>
+      <c r="E72" s="32"/>
+      <c r="M72" s="24"/>
+      <c r="N72" s="32"/>
+      <c r="Q72" s="24"/>
+      <c r="R72" s="33"/>
+      <c r="U72" s="30"/>
+      <c r="V72" s="19"/>
+    </row>
+    <row r="73" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D73" s="24"/>
+      <c r="E73" s="32"/>
+      <c r="M73" s="24"/>
+      <c r="N73" s="32"/>
+      <c r="Q73" s="24"/>
+      <c r="R73" s="33"/>
+      <c r="U73" s="30"/>
+      <c r="V73" s="19"/>
+    </row>
+    <row r="74" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D74" s="24"/>
+      <c r="E74" s="32"/>
+      <c r="M74" s="24"/>
+      <c r="N74" s="32"/>
+      <c r="Q74" s="24"/>
+      <c r="R74" s="33"/>
+      <c r="U74" s="30"/>
+      <c r="V74" s="19"/>
+    </row>
+    <row r="75" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D75" s="24"/>
+      <c r="E75" s="32"/>
+      <c r="M75" s="24"/>
+      <c r="N75" s="32"/>
+      <c r="Q75" s="24"/>
+      <c r="R75" s="33"/>
+      <c r="U75" s="30"/>
+      <c r="V75" s="19"/>
+    </row>
+    <row r="76" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D76" s="24"/>
+      <c r="E76" s="32"/>
+      <c r="M76" s="24"/>
+      <c r="N76" s="32"/>
+      <c r="Q76" s="24"/>
+      <c r="R76" s="33"/>
+      <c r="U76" s="30"/>
+      <c r="V76" s="19"/>
+    </row>
+    <row r="77" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D77" s="24"/>
+      <c r="E77" s="32"/>
+      <c r="M77" s="24"/>
+      <c r="N77" s="32"/>
+      <c r="Q77" s="24"/>
+      <c r="R77" s="33"/>
+      <c r="U77" s="30"/>
+      <c r="V77" s="19"/>
+    </row>
+    <row r="78" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D78" s="24"/>
+      <c r="E78" s="32"/>
+      <c r="M78" s="24"/>
+      <c r="N78" s="32"/>
+      <c r="Q78" s="24"/>
+      <c r="R78" s="33"/>
+      <c r="U78" s="30"/>
+      <c r="V78" s="19"/>
+    </row>
+    <row r="79" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D79" s="24"/>
+      <c r="E79" s="32"/>
+      <c r="M79" s="24"/>
+      <c r="N79" s="32"/>
+      <c r="Q79" s="24"/>
+      <c r="R79" s="33"/>
+      <c r="U79" s="30"/>
+      <c r="V79" s="19"/>
+    </row>
+    <row r="80" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D80" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E80" s="32">
+        <v>5</v>
+      </c>
+      <c r="M80" s="24"/>
+      <c r="N80" s="32"/>
+      <c r="Q80" s="24"/>
+      <c r="R80" s="33"/>
+    </row>
+    <row r="81" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D81" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E81" s="32">
+        <v>65</v>
+      </c>
+      <c r="M81" s="24"/>
+    </row>
+    <row r="82" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D82" s="24"/>
+      <c r="E82" s="32"/>
+    </row>
+    <row r="83" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D83" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E56" s="32">
+      <c r="E83" s="32">
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="24" t="s">
+    <row r="84" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D84" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="E57" s="32">
+      <c r="E84" s="32">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="24" t="s">
+    <row r="85" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D85" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="E58" s="32">
+      <c r="E85" s="32">
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="24" t="s">
+    <row r="86" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D86" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="E59" s="32">
+      <c r="E86" s="32">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="24" t="s">
+    <row r="87" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D87" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="E60" s="32">
+      <c r="E87" s="32">
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D61" s="24" t="s">
+    <row r="88" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D88" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="E61" s="32">
+      <c r="E88" s="32">
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="24" t="s">
+    <row r="89" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D89" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="E62" s="32">
+      <c r="E89" s="32">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="24" t="s">
+    <row r="90" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D90" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="E63" s="32">
+      <c r="E90" s="32">
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="24" t="s">
+    <row r="91" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D91" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="E64" s="32">
+      <c r="E91" s="32">
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="24" t="s">
+    <row r="92" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D92" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="E65" s="32">
+      <c r="E92" s="32">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="24" t="s">
+    <row r="93" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D93" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E66" s="32">
+      <c r="E93" s="32">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D67" s="24" t="s">
+    <row r="94" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D94" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="E67" s="32">
+      <c r="E94" s="32">
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D68" s="24" t="s">
+    <row r="95" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D95" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="E68" s="32">
+      <c r="E95" s="32">
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D69" s="24" t="s">
+    <row r="96" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D96" s="24" t="s">
         <v>114</v>
-      </c>
-      <c r="E69" s="32">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="E70" s="32">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="71" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="E71" s="32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="72" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D72" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="E72" s="32">
-        <v>49.95</v>
-      </c>
-    </row>
-    <row r="73" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D73" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="E73" s="32">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="74" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D74" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="E74" s="32">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="75" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D75" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="E75" s="32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="76" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D76" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E76" s="32">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="77" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D77" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="E77" s="32">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="78" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D78" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="E78" s="32">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="79" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D79" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E79" s="32">
-        <v>1.31</v>
-      </c>
-    </row>
-    <row r="80" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D80" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="E80" s="32">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="81" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D81" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="E81" s="32">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="82" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D82" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="E82" s="32">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="83" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D83" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="E83" s="32">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="84" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D84" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="E84" s="32">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="85" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D85" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="E85" s="32">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="86" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D86" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E86" s="32">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="87" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D87" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E87" s="32">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="88" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D88" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="E88" s="32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D89" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="E89" s="32">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="90" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D90" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E90" s="32">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="91" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D91" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="E91" s="32">
-        <v>431.42</v>
-      </c>
-    </row>
-    <row r="92" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D92" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="E92" s="32">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="93" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D93" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="E93" s="32">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="94" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D94" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="E94" s="32">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="95" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D95" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E95" s="32">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="96" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D96" s="24" t="s">
-        <v>150</v>
       </c>
       <c r="E96" s="32">
         <v>50</v>
@@ -6815,122 +6979,338 @@
     </row>
     <row r="97" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D97" s="24" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
       <c r="E97" s="32">
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D98" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E98" s="32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="99" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D99" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E99" s="32">
+        <v>49.95</v>
+      </c>
+    </row>
     <row r="100" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D100" s="24" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="E100" s="32">
-        <v>503</v>
+        <v>308</v>
       </c>
     </row>
     <row r="101" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D101" s="24" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="E101" s="32">
-        <v>320</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D102" s="24" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="E102" s="32">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="103" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D103" s="24" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E103" s="32">
-        <v>65</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D104" s="24" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="E104" s="32">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="105" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D105" s="24" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="E105" s="32">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="106" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D106" s="24" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="E106" s="32">
-        <v>25</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="107" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D107" s="24" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="E107" s="32">
-        <v>431.42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="108" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D108" s="24" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E108" s="32">
-        <v>360</v>
+        <v>50</v>
       </c>
     </row>
     <row r="109" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D109" s="24" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="E109" s="32">
-        <v>25</v>
+        <v>85</v>
       </c>
     </row>
     <row r="110" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D110" s="24" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="E110" s="32">
-        <v>65</v>
+        <v>440</v>
       </c>
     </row>
     <row r="111" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D111" s="24" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="E111" s="32">
-        <v>25</v>
+        <v>503</v>
       </c>
     </row>
     <row r="112" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D112" s="24" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="E112" s="32">
-        <v>50</v>
+        <v>320</v>
       </c>
     </row>
     <row r="113" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D113" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E113" s="32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D114" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E114" s="32">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="115" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D115" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E115" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D116" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E116" s="32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="117" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D117" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E117" s="32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D118" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E118" s="32">
+        <v>431.42</v>
+      </c>
+    </row>
+    <row r="119" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D119" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="E119" s="32">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D120" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E120" s="32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D121" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E121" s="32">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="122" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D122" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E122" s="32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="123" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D123" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E123" s="32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="124" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D124" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="E113" s="32">
+      <c r="E124" s="32">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="126" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D127" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E127" s="32">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="128" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D128" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E128" s="32">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D129" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E129" s="32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D130" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E130" s="32">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D131" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E131" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D132" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E132" s="32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D133" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E133" s="32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="134" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D134" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E134" s="32">
+        <v>431.42</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D135" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="E135" s="32">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="136" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D136" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E136" s="32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="137" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D137" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E137" s="32">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="138" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D138" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E138" s="32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="139" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D139" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E139" s="32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="140" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D140" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="E140" s="32">
         <v>40</v>
       </c>
     </row>
@@ -6950,8 +7330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>